<commit_message>
Improve Look & Feel
</commit_message>
<xml_diff>
--- a/src/assets/hours/UTN.xlsx
+++ b/src/assets/hours/UTN.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas Pochettino\source\repos\Angular-UTN-Monitor\src\assets\hours\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD0DE7FA-C696-4EEB-A897-2DDFEC694DE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{099B1E4C-5403-43C8-A584-CF5A102AFCA8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1011,7 +1011,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1058,6 +1058,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -1279,13 +1283,14 @@
   </sheetPr>
   <dimension ref="A1:H148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="A147" sqref="A147"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C89" sqref="C89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.109375" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" style="49"/>
     <col min="5" max="5" width="12.77734375" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.44140625" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="39.6640625" bestFit="1" customWidth="1"/>
@@ -1299,7 +1304,7 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="46" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -2086,7 +2091,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>6</v>
       </c>
@@ -2110,7 +2115,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>6</v>
       </c>
@@ -2134,7 +2139,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>6</v>
       </c>
@@ -2158,7 +2163,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>6</v>
       </c>
@@ -2182,7 +2187,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
         <v>6</v>
       </c>
@@ -2206,7 +2211,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>6</v>
       </c>
@@ -2230,7 +2235,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>6</v>
       </c>
@@ -2254,7 +2259,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>6</v>
       </c>
@@ -2278,7 +2283,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>6</v>
       </c>
@@ -2302,7 +2307,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>6</v>
       </c>
@@ -2326,7 +2331,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
         <v>6</v>
       </c>
@@ -2350,7 +2355,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
         <v>60</v>
       </c>
@@ -2374,7 +2379,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="30" t="s">
         <v>60</v>
       </c>
@@ -2398,7 +2403,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
         <v>60</v>
       </c>
@@ -2422,7 +2427,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
         <v>60</v>
       </c>
@@ -2446,7 +2451,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
         <v>60</v>
       </c>
@@ -2470,7 +2475,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
         <v>60</v>
       </c>
@@ -2494,7 +2499,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
         <v>60</v>
       </c>
@@ -2518,7 +2523,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
         <v>60</v>
       </c>
@@ -2542,7 +2547,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
         <v>61</v>
       </c>
@@ -2566,7 +2571,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
         <v>61</v>
       </c>
@@ -2590,7 +2595,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
         <v>61</v>
       </c>
@@ -2614,7 +2619,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>61</v>
       </c>
@@ -2638,7 +2643,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
         <v>61</v>
       </c>
@@ -2662,7 +2667,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
         <v>61</v>
       </c>
@@ -2686,7 +2691,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="10" t="s">
         <v>62</v>
       </c>
@@ -2710,7 +2715,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="10" t="s">
         <v>62</v>
       </c>
@@ -2734,7 +2739,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="11" t="s">
         <v>162</v>
       </c>
@@ -2758,7 +2763,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="11" t="s">
         <v>162</v>
       </c>
@@ -2782,7 +2787,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="11" t="s">
         <v>162</v>
       </c>
@@ -2811,9 +2816,11 @@
         <v>37</v>
       </c>
       <c r="B64" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C64" s="20"/>
+        <v>54</v>
+      </c>
+      <c r="C64" s="47">
+        <v>44224</v>
+      </c>
       <c r="D64" s="20" t="s">
         <v>38</v>
       </c>
@@ -3406,14 +3413,14 @@
         <v>104</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="20" t="s">
         <v>37</v>
       </c>
       <c r="B89" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="C89" s="20"/>
+      <c r="C89" s="47"/>
       <c r="D89" s="20" t="s">
         <v>38</v>
       </c>
@@ -3430,16 +3437,14 @@
         <v>46</v>
       </c>
     </row>
-    <row r="90" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="12" t="s">
         <v>37</v>
       </c>
       <c r="B90" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="C90" s="15">
-        <v>44056</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="C90" s="15"/>
       <c r="D90" s="12" t="s">
         <v>38</v>
       </c>
@@ -3816,14 +3821,14 @@
         <v>193</v>
       </c>
     </row>
-    <row r="106" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="20" t="s">
         <v>37</v>
       </c>
       <c r="B106" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="C106" s="20"/>
+      <c r="C106" s="47"/>
       <c r="D106" s="20" t="s">
         <v>38</v>
       </c>
@@ -4104,7 +4109,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="118" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="7" t="s">
         <v>6</v>
       </c>
@@ -4128,7 +4133,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="119" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="7" t="s">
         <v>6</v>
       </c>
@@ -4152,7 +4157,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="120" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="7" t="s">
         <v>6</v>
       </c>
@@ -4176,7 +4181,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="121" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="7" t="s">
         <v>6</v>
       </c>
@@ -4200,7 +4205,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="122" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="7" t="s">
         <v>6</v>
       </c>
@@ -4224,7 +4229,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="123" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="7" t="s">
         <v>6</v>
       </c>
@@ -4248,7 +4253,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="124" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="7" t="s">
         <v>6</v>
       </c>
@@ -4272,7 +4277,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="125" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="7" t="s">
         <v>6</v>
       </c>
@@ -4296,7 +4301,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="126" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="7" t="s">
         <v>6</v>
       </c>
@@ -4320,7 +4325,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="127" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="7" t="s">
         <v>6</v>
       </c>
@@ -4344,7 +4349,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="128" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="7" t="s">
         <v>6</v>
       </c>
@@ -4368,7 +4373,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="129" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="7" t="s">
         <v>6</v>
       </c>
@@ -4392,7 +4397,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="130" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="7" t="s">
         <v>6</v>
       </c>
@@ -4416,7 +4421,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="131" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="8" t="s">
         <v>60</v>
       </c>
@@ -4440,7 +4445,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="132" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="8" t="s">
         <v>60</v>
       </c>
@@ -4464,7 +4469,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="133" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="8" t="s">
         <v>60</v>
       </c>
@@ -4488,7 +4493,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="134" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="8" t="s">
         <v>60</v>
       </c>
@@ -4512,7 +4517,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="135" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="8" t="s">
         <v>60</v>
       </c>
@@ -4536,7 +4541,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="136" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="8" t="s">
         <v>60</v>
       </c>
@@ -4560,7 +4565,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="137" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="8" t="s">
         <v>60</v>
       </c>
@@ -4584,7 +4589,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="138" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="8" t="s">
         <v>60</v>
       </c>
@@ -4608,7 +4613,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="139" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="8" t="s">
         <v>60</v>
       </c>
@@ -4632,7 +4637,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="140" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="9" t="s">
         <v>61</v>
       </c>
@@ -4656,7 +4661,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="141" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="9" t="s">
         <v>61</v>
       </c>
@@ -4680,7 +4685,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="142" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="9" t="s">
         <v>61</v>
       </c>
@@ -4704,7 +4709,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="143" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="10" t="s">
         <v>62</v>
       </c>
@@ -4728,7 +4733,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="144" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="10" t="s">
         <v>62</v>
       </c>
@@ -4752,7 +4757,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="145" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="38" t="s">
         <v>162</v>
       </c>
@@ -4776,7 +4781,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="146" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="38" t="s">
         <v>162</v>
       </c>
@@ -4807,7 +4812,7 @@
       <c r="B147" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="C147" s="42"/>
+      <c r="C147" s="48"/>
       <c r="D147" s="42" t="s">
         <v>38</v>
       </c>
@@ -4831,7 +4836,7 @@
       <c r="B148" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="C148" s="42"/>
+      <c r="C148" s="48"/>
       <c r="D148" s="42" t="s">
         <v>38</v>
       </c>
@@ -4850,10 +4855,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:H148" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <filterColumn colId="1">
+    <filterColumn colId="0">
       <filters>
-        <filter val="Lunes"/>
-        <filter val="Martes"/>
+        <filter val="Auditorium"/>
       </filters>
     </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H117">

</xml_diff>